<commit_message>
update on 2016.12.22 for data
</commit_message>
<xml_diff>
--- a/microblog/data.xlsx
+++ b/microblog/data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="1" r:id="rId1"/>
@@ -16,13 +16,14 @@
     <sheet name="Service" sheetId="7" r:id="rId7"/>
     <sheet name="Daily tool" sheetId="8" r:id="rId8"/>
     <sheet name="Special setup" sheetId="9" r:id="rId9"/>
+    <sheet name="Standard TB" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="521">
   <si>
     <t>Name</t>
   </si>
@@ -1145,7 +1146,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1166,7 +1167,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1187,7 +1188,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1208,7 +1209,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1229,7 +1230,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1268,7 +1269,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1282,9 +1283,6 @@
     <t>iSCSI Ports</t>
   </si>
   <si>
-    <t>SanBlaze IP/Port assignment</t>
-  </si>
-  <si>
     <t>Data Mobility</t>
   </si>
   <si>
@@ -1663,17 +1661,45 @@
   </si>
   <si>
     <t>Bonn Liu</t>
+  </si>
+  <si>
+    <t>SanBlaze Type</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>SanBlaze IP</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>SanBlaze Port</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Name</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>Password</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>vlun</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sanblaze</t>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1688,21 +1714,21 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF1F497D"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1717,7 +1743,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1757,7 +1783,7 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1772,6 +1798,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -2024,7 +2057,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2123,23 +2156,32 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2160,7 +2202,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2202,7 +2244,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2235,9 +2277,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2270,6 +2329,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2452,9 +2528,12 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2492,7 +2571,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="14.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2524,7 +2603,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="14.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2556,7 +2635,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="14.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2588,7 +2667,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="14.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2620,7 +2699,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="14.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -2658,7 +2737,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="14.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -2696,7 +2775,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="14.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -2734,7 +2813,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="14.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -2772,7 +2851,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="14.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -2810,7 +2889,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="14.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -2848,7 +2927,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="14.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>81</v>
       </c>
@@ -2886,7 +2965,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="14.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>89</v>
       </c>
@@ -2924,7 +3003,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="14.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>97</v>
       </c>
@@ -2962,7 +3041,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="14.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>105</v>
       </c>
@@ -3000,7 +3079,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="14.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>112</v>
       </c>
@@ -3038,7 +3117,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="14.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>119</v>
       </c>
@@ -3076,7 +3155,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="14.45">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>127</v>
       </c>
@@ -3114,7 +3193,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="14.45">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>134</v>
       </c>
@@ -3152,7 +3231,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="14.45">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>141</v>
       </c>
@@ -3190,7 +3269,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="14.45">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>148</v>
       </c>
@@ -3228,7 +3307,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="14.45">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>155</v>
       </c>
@@ -3254,7 +3333,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="14.45">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>162</v>
       </c>
@@ -3280,7 +3359,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>167</v>
       </c>
@@ -3306,7 +3385,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>172</v>
       </c>
@@ -3332,7 +3411,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>177</v>
       </c>
@@ -3364,7 +3443,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>182</v>
       </c>
@@ -3398,7 +3477,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>187</v>
       </c>
@@ -3432,7 +3511,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>192</v>
       </c>
@@ -3467,6 +3546,21 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="15" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3479,14 +3573,15 @@
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3503,7 +3598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>199</v>
       </c>
@@ -3520,7 +3615,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>203</v>
       </c>
@@ -3534,7 +3629,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>206</v>
       </c>
@@ -3551,7 +3646,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>209</v>
       </c>
@@ -3565,7 +3660,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>211</v>
       </c>
@@ -3579,7 +3674,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>214</v>
       </c>
@@ -3596,7 +3691,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>216</v>
       </c>
@@ -3610,7 +3705,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>218</v>
       </c>
@@ -3627,7 +3722,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>220</v>
       </c>
@@ -3644,7 +3739,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>222</v>
       </c>
@@ -3658,7 +3753,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>224</v>
       </c>
@@ -3675,7 +3770,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>227</v>
       </c>
@@ -3692,7 +3787,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>229</v>
       </c>
@@ -3709,7 +3804,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>231</v>
       </c>
@@ -3726,7 +3821,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>233</v>
       </c>
@@ -3740,7 +3835,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>235</v>
       </c>
@@ -3757,7 +3852,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>237</v>
       </c>
@@ -3774,7 +3869,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>239</v>
       </c>
@@ -3788,7 +3883,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>241</v>
       </c>
@@ -3802,7 +3897,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>243</v>
       </c>
@@ -3819,7 +3914,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>245</v>
       </c>
@@ -3836,7 +3931,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>247</v>
       </c>
@@ -3853,7 +3948,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>249</v>
       </c>
@@ -3870,7 +3965,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>251</v>
       </c>
@@ -3884,7 +3979,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>253</v>
       </c>
@@ -3898,7 +3993,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>255</v>
       </c>
@@ -3915,7 +4010,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>258</v>
       </c>
@@ -3932,7 +4027,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>260</v>
       </c>
@@ -3949,7 +4044,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>262</v>
       </c>
@@ -3966,7 +4061,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>264</v>
       </c>
@@ -3983,7 +4078,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>266</v>
       </c>
@@ -4000,7 +4095,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>268</v>
       </c>
@@ -4014,7 +4109,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>270</v>
       </c>
@@ -4028,7 +4123,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>272</v>
       </c>
@@ -4045,7 +4140,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>274</v>
       </c>
@@ -4062,7 +4157,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>276</v>
       </c>
@@ -4079,7 +4174,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>278</v>
       </c>
@@ -4096,7 +4191,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>280</v>
       </c>
@@ -4113,7 +4208,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>282</v>
       </c>
@@ -4130,7 +4225,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>284</v>
       </c>
@@ -4147,7 +4242,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>286</v>
       </c>
@@ -4164,7 +4259,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>288</v>
       </c>
@@ -4181,7 +4276,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>290</v>
       </c>
@@ -4198,7 +4293,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>292</v>
       </c>
@@ -4212,7 +4307,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>294</v>
       </c>
@@ -4229,7 +4324,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>296</v>
       </c>
@@ -4246,7 +4341,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>298</v>
       </c>
@@ -4263,7 +4358,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>300</v>
       </c>
@@ -4280,7 +4375,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>302</v>
       </c>
@@ -4297,7 +4392,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>304</v>
       </c>
@@ -4314,7 +4409,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
         <v>306</v>
       </c>
@@ -4331,7 +4426,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
         <v>308</v>
       </c>
@@ -4348,7 +4443,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
         <v>310</v>
       </c>
@@ -4365,7 +4460,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
         <v>312</v>
       </c>
@@ -4376,7 +4471,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
         <v>313</v>
       </c>
@@ -4393,7 +4488,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
         <v>315</v>
       </c>
@@ -4410,7 +4505,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
         <v>317</v>
       </c>
@@ -4427,7 +4522,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
         <v>319</v>
       </c>
@@ -4444,7 +4539,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
         <v>321</v>
       </c>
@@ -4461,7 +4556,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
         <v>323</v>
       </c>
@@ -4479,6 +4574,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4491,16 +4587,16 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4523,7 +4619,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1">
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>331</v>
       </c>
@@ -4537,7 +4633,7 @@
         <v>334</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>335</v>
@@ -4546,21 +4642,21 @@
         <v>336</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>337</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>338</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>335</v>
@@ -4569,21 +4665,21 @@
         <v>336</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>414</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>416</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>417</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>335</v>
@@ -4592,21 +4688,21 @@
         <v>336</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>419</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>421</v>
-      </c>
       <c r="E5" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>339</v>
@@ -4615,7 +4711,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>341</v>
       </c>
@@ -4623,13 +4719,13 @@
         <v>342</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>339</v>
@@ -4638,21 +4734,21 @@
         <v>340</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>343</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>416</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>417</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>339</v>
@@ -4661,12 +4757,12 @@
         <v>336</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1">
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>423</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>424</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>344</v>
@@ -4678,13 +4774,13 @@
         <v>345</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>346</v>
       </c>
@@ -4692,7 +4788,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>338</v>
@@ -4704,10 +4800,10 @@
         <v>349</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>218</v>
       </c>
@@ -4721,7 +4817,7 @@
         <v>338</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>219</v>
@@ -4730,7 +4826,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>214</v>
       </c>
@@ -4744,62 +4840,63 @@
         <v>338</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F11" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>428</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A12" t="s">
+      <c r="B12" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>430</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>338</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1">
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>338</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>336</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="15" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1"/>
     <hyperlink ref="G7" r:id="rId2"/>
@@ -4822,15 +4919,16 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>350</v>
       </c>
@@ -4853,7 +4951,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -4876,7 +4974,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -4899,7 +4997,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -4922,7 +5020,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -4945,7 +5043,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -4968,7 +5066,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -4991,7 +5089,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>192</v>
       </c>
@@ -5014,7 +5112,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
         <v>192</v>
       </c>
@@ -5037,7 +5135,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
         <v>386</v>
       </c>
@@ -5054,7 +5152,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
         <v>37</v>
       </c>
@@ -5073,7 +5171,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>192</v>
       </c>
@@ -5096,30 +5194,35 @@
         <v>362</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="F16" s="9"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
         <v>392</v>
       </c>
@@ -5130,12 +5233,22 @@
         <v>393</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>394</v>
-      </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1">
+        <v>514</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>515</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="G1" s="49" t="s">
+        <v>517</v>
+      </c>
+      <c r="H1" s="49" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>112</v>
       </c>
@@ -5143,39 +5256,51 @@
         <v>30</v>
       </c>
       <c r="C2" s="19" t="s">
+        <v>394</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>395</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="E2" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>397</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="G2" s="20" t="s">
+        <v>519</v>
+      </c>
+      <c r="H2" s="50" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
         <v>398</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A3" s="18" t="s">
-        <v>399</v>
       </c>
       <c r="B3" s="20" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="20" t="s">
+        <v>394</v>
+      </c>
+      <c r="D3" s="20" t="s">
         <v>395</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>396</v>
-      </c>
       <c r="E3" s="20" t="s">
+        <v>399</v>
+      </c>
+      <c r="F3" s="20" t="s">
         <v>400</v>
       </c>
-      <c r="F3" s="20" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1">
+      <c r="G3" s="20" t="s">
+        <v>519</v>
+      </c>
+      <c r="H3" s="50" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>42</v>
       </c>
@@ -5183,19 +5308,25 @@
         <v>30</v>
       </c>
       <c r="C4" s="20" t="s">
+        <v>394</v>
+      </c>
+      <c r="D4" s="20" t="s">
         <v>395</v>
       </c>
-      <c r="D4" s="20" t="s">
-        <v>396</v>
-      </c>
       <c r="E4" s="20" t="s">
+        <v>401</v>
+      </c>
+      <c r="F4" s="20" t="s">
         <v>402</v>
       </c>
-      <c r="F4" s="20" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1">
+      <c r="G4" s="20" t="s">
+        <v>519</v>
+      </c>
+      <c r="H4" s="50" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>53</v>
       </c>
@@ -5203,39 +5334,52 @@
         <v>30</v>
       </c>
       <c r="C5" s="20" t="s">
+        <v>394</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>395</v>
       </c>
-      <c r="D5" s="20" t="s">
-        <v>396</v>
-      </c>
       <c r="E5" s="21" t="s">
+        <v>403</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>404</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="G5" s="21" t="s">
+        <v>519</v>
+      </c>
+      <c r="H5" s="50" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
         <v>405</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A6" s="18" t="s">
-        <v>406</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="20" t="s">
+        <v>394</v>
+      </c>
+      <c r="D6" s="20" t="s">
         <v>395</v>
       </c>
-      <c r="D6" s="20" t="s">
-        <v>396</v>
-      </c>
       <c r="E6" s="20" t="s">
+        <v>406</v>
+      </c>
+      <c r="F6" s="20" t="s">
         <v>407</v>
       </c>
-      <c r="F6" s="20" t="s">
-        <v>408</v>
+      <c r="G6" s="20" t="s">
+        <v>519</v>
+      </c>
+      <c r="H6" s="50" t="s">
+        <v>520</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="15" type="noConversion"/>
   <conditionalFormatting sqref="E1:F1">
     <cfRule type="dataBar" priority="1">
       <dataBar>
@@ -5281,35 +5425,38 @@
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="45.75" thickBot="1">
+    <row r="1" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
+        <v>432</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>433</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="C1" s="23" t="s">
         <v>434</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="D1" s="23" t="s">
         <v>435</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="E1" s="23" t="s">
         <v>436</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="F1" s="23" t="s">
         <v>437</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="G1" s="23" t="s">
         <v>438</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="H1" s="23" t="s">
         <v>439</v>
       </c>
-      <c r="H1" s="23" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24">
         <v>1</v>
       </c>
@@ -5317,7 +5464,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D2" s="27">
         <v>3</v>
@@ -5329,13 +5476,13 @@
         <v>1</v>
       </c>
       <c r="G2" s="27" t="s">
+        <v>441</v>
+      </c>
+      <c r="H2" s="27" t="s">
         <v>442</v>
       </c>
-      <c r="H2" s="27" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1">
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24">
         <v>2</v>
       </c>
@@ -5343,7 +5490,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D3" s="27">
         <v>3</v>
@@ -5355,13 +5502,13 @@
         <v>1</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="28">
         <v>7</v>
       </c>
@@ -5369,7 +5516,7 @@
         <v>192</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D4" s="27">
         <v>3</v>
@@ -5381,13 +5528,14 @@
         <v>0</v>
       </c>
       <c r="G4" s="27" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H4" s="27" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="15" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" location="systemDetails::storagesystem=FNM00124100004" display="https://portal.usd.lab.emc.com/services/equipment_management - systemDetails::storagesystem=FNM00124100004"/>
     <hyperlink ref="B3" r:id="rId2" location="systemDetails::storagesystem=FNM00124400703" display="https://portal.usd.lab.emc.com/services/equipment_management - systemDetails::storagesystem=FNM00124400703"/>
@@ -5405,27 +5553,27 @@
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="31" t="s">
+        <v>446</v>
+      </c>
+      <c r="B1" s="32" t="s">
         <v>447</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="C1" s="32" t="s">
         <v>448</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="D1" s="32" t="s">
         <v>449</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>450</v>
       </c>
       <c r="E1" s="32" t="s">
         <v>352</v>
@@ -5434,119 +5582,119 @@
         <v>327</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
+        <v>450</v>
+      </c>
+      <c r="B2" s="32" t="s">
         <v>451</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="C2" s="32" t="s">
         <v>452</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="D2" s="34" t="s">
         <v>453</v>
       </c>
-      <c r="D2" s="34" t="s">
-        <v>454</v>
-      </c>
       <c r="E2" s="35" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F2" s="33" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="31" t="s">
+        <v>454</v>
+      </c>
+      <c r="B3" s="35" t="s">
         <v>455</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="C3" s="35" t="s">
         <v>456</v>
-      </c>
-      <c r="C3" s="35" t="s">
-        <v>457</v>
       </c>
       <c r="D3" s="32"/>
       <c r="E3" s="35" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F3" s="33" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="31" t="s">
+        <v>458</v>
+      </c>
+      <c r="B4" s="32" t="s">
         <v>459</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="C4" s="32" t="s">
         <v>460</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>461</v>
       </c>
       <c r="D4" s="32"/>
       <c r="E4" s="32"/>
       <c r="F4" s="33"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
+        <v>461</v>
+      </c>
+      <c r="B5" s="32" t="s">
         <v>462</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="C5" s="36" t="s">
         <v>463</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="D5" s="32" t="s">
         <v>464</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>465</v>
       </c>
       <c r="E5" s="32"/>
       <c r="F5" s="33"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="31" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B6" s="32" t="s">
+        <v>459</v>
+      </c>
+      <c r="C6" s="32" t="s">
         <v>460</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>461</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="32"/>
       <c r="F6" s="33"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="31" t="s">
+        <v>466</v>
+      </c>
+      <c r="B7" s="32" t="s">
         <v>467</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="C7" s="32" t="s">
         <v>468</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>469</v>
       </c>
       <c r="D7" s="32"/>
       <c r="E7" s="32"/>
       <c r="F7" s="33"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="31" t="s">
+        <v>469</v>
+      </c>
+      <c r="B8" s="32" t="s">
         <v>470</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="C8" s="32" t="s">
         <v>471</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>472</v>
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="32"/>
       <c r="F8" s="33"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="31" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B9" s="32"/>
       <c r="C9" s="32"/>
@@ -5554,9 +5702,9 @@
       <c r="E9" s="32"/>
       <c r="F9" s="33"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="31" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B10" s="32"/>
       <c r="C10" s="32"/>
@@ -5564,13 +5712,13 @@
       <c r="E10" s="32"/>
       <c r="F10" s="33"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="31" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B11" s="32"/>
       <c r="C11" s="32" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D11" s="32"/>
       <c r="E11" s="37" t="s">
@@ -5580,21 +5728,22 @@
         <v>338</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="38" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B12" s="39" t="s">
+        <v>476</v>
+      </c>
+      <c r="C12" s="40" t="s">
         <v>477</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>478</v>
       </c>
       <c r="D12" s="40"/>
       <c r="E12" s="40"/>
       <c r="F12" s="41"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5607,20 +5756,21 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="134.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="134.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C1" t="s">
         <v>352</v>
@@ -5629,15 +5779,15 @@
         <v>327</v>
       </c>
       <c r="E1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>480</v>
-      </c>
-      <c r="B2" t="s">
-        <v>481</v>
       </c>
       <c r="C2" s="42" t="s">
         <v>333</v>
@@ -5646,81 +5796,82 @@
         <v>338</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>481</v>
+      </c>
+      <c r="B3" t="s">
         <v>482</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>483</v>
-      </c>
-      <c r="C3" t="s">
-        <v>484</v>
       </c>
       <c r="D3" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B4" s="43" t="s">
         <v>228</v>
       </c>
       <c r="C4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E4" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+      <c r="B5" s="44" t="s">
         <v>487</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="C5" t="s">
         <v>488</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>490</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>492</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>494</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>496</v>
       </c>
-      <c r="B9" t="s">
-        <v>497</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="15" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1"/>
   </hyperlinks>
@@ -5735,19 +5886,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="73" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="45" t="s">
         <v>392</v>
       </c>
@@ -5755,41 +5906,41 @@
         <v>5</v>
       </c>
       <c r="C1" s="45" t="s">
+        <v>498</v>
+      </c>
+      <c r="D1" s="45" t="s">
         <v>499</v>
       </c>
-      <c r="D1" s="45" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="45" t="s">
         <v>53</v>
       </c>
       <c r="B2" s="45" t="s">
+        <v>500</v>
+      </c>
+      <c r="C2" s="45" t="s">
         <v>501</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="D2" s="45" t="s">
         <v>502</v>
       </c>
-      <c r="D2" s="45" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+    </row>
+    <row r="3" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="45" t="s">
         <v>134</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="46" t="s">
-        <v>504</v>
-      </c>
-      <c r="D3" s="47" t="s">
+      <c r="C3" s="47" t="s">
+        <v>503</v>
+      </c>
+      <c r="D3" s="46" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="45" t="s">
         <v>141</v>
       </c>
@@ -5801,154 +5952,155 @@
         <v>349</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="45" t="s">
         <v>42</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C5" s="45"/>
       <c r="D5" s="45" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="45" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="45" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C6" s="45"/>
       <c r="D6" s="45" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="45" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="45" t="s">
-        <v>508</v>
-      </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47" t="s">
+        <v>507</v>
+      </c>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="45" t="s">
         <v>148</v>
       </c>
       <c r="B8" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="47"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="45" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="45" t="s">
         <v>58</v>
       </c>
       <c r="B9" s="45" t="s">
-        <v>508</v>
-      </c>
-      <c r="C9" s="47"/>
+        <v>507</v>
+      </c>
+      <c r="C9" s="46"/>
       <c r="D9" s="45" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="45" t="s">
         <v>81</v>
       </c>
       <c r="B10" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="47"/>
+      <c r="C10" s="46"/>
       <c r="D10" s="45" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="45" t="s">
         <v>89</v>
       </c>
       <c r="B11" s="45" t="s">
-        <v>511</v>
-      </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="45" t="s">
         <v>97</v>
       </c>
       <c r="B12" s="45" t="s">
-        <v>512</v>
-      </c>
-      <c r="C12" s="47"/>
+        <v>511</v>
+      </c>
+      <c r="C12" s="46"/>
       <c r="D12" s="45" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" s="45" t="s">
         <v>105</v>
       </c>
       <c r="B13" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47" t="s">
+      <c r="C13" s="46"/>
+      <c r="D13" s="46" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="45" t="s">
         <v>112</v>
       </c>
       <c r="B14" s="45" t="s">
+        <v>511</v>
+      </c>
+      <c r="C14" s="46"/>
+      <c r="D14" s="45" t="s">
         <v>512</v>
       </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="45" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+    </row>
+    <row r="15" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" s="45" t="s">
         <v>119</v>
       </c>
       <c r="B15" s="45" t="s">
-        <v>514</v>
-      </c>
-      <c r="C15" s="47"/>
+        <v>513</v>
+      </c>
+      <c r="C15" s="46"/>
       <c r="D15" s="45" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="45" t="s">
         <v>127</v>
       </c>
       <c r="B16" s="45" t="s">
-        <v>512</v>
-      </c>
-      <c r="C16" s="47"/>
+        <v>511</v>
+      </c>
+      <c r="C16" s="46"/>
       <c r="D16" s="45" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C3:C4"/>
   </mergeCells>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add upload file module
</commit_message>
<xml_diff>
--- a/microblog/data.xlsx
+++ b/microblog/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="1" r:id="rId1"/>
@@ -2157,17 +2157,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3556,9 +3556,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+  </cols>
   <sheetData/>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3569,7 +3572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
@@ -4584,7 +4587,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4872,7 +4875,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>428</v>
       </c>
@@ -4908,6 +4911,7 @@
     <hyperlink ref="G12" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -5207,8 +5211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5241,10 +5245,10 @@
       <c r="F1" s="17" t="s">
         <v>516</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="47" t="s">
         <v>517</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="47" t="s">
         <v>518</v>
       </c>
     </row>
@@ -5270,7 +5274,7 @@
       <c r="G2" s="20" t="s">
         <v>519</v>
       </c>
-      <c r="H2" s="50" t="s">
+      <c r="H2" s="48" t="s">
         <v>520</v>
       </c>
     </row>
@@ -5296,7 +5300,7 @@
       <c r="G3" s="20" t="s">
         <v>519</v>
       </c>
-      <c r="H3" s="50" t="s">
+      <c r="H3" s="48" t="s">
         <v>520</v>
       </c>
     </row>
@@ -5322,7 +5326,7 @@
       <c r="G4" s="20" t="s">
         <v>519</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="48" t="s">
         <v>520</v>
       </c>
     </row>
@@ -5348,7 +5352,7 @@
       <c r="G5" s="21" t="s">
         <v>519</v>
       </c>
-      <c r="H5" s="50" t="s">
+      <c r="H5" s="48" t="s">
         <v>520</v>
       </c>
     </row>
@@ -5374,7 +5378,7 @@
       <c r="G6" s="20" t="s">
         <v>519</v>
       </c>
-      <c r="H6" s="50" t="s">
+      <c r="H6" s="48" t="s">
         <v>520</v>
       </c>
     </row>
@@ -5549,7 +5553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -5933,7 +5937,7 @@
       <c r="B3" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="49" t="s">
         <v>503</v>
       </c>
       <c r="D3" s="46" t="s">
@@ -5947,7 +5951,7 @@
       <c r="B4" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="48"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="45" t="s">
         <v>349</v>
       </c>

</xml_diff>